<commit_message>
add new methods to WasteStream, update Toilet and PitLatrine
</commit_message>
<xml_diff>
--- a/sanitation/systems/bwaise/inputs/units.xlsx
+++ b/sanitation/systems/bwaise/inputs/units.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfca01abaf64aab7/Coding/sanitation_Yalin/sanitation/systems/bwaise/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="534" documentId="8_{DCECA136-6458-0041-B737-5433DA0EAABB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0C1F3038-9DD2-7F4D-864C-8C76FE4D26F7}"/>
+  <xr:revisionPtr revIDLastSave="561" documentId="8_{DCECA136-6458-0041-B737-5433DA0EAABB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E693DE9D-A6B5-764A-AFF2-2349CC8483AE}"/>
   <bookViews>
-    <workbookView xWindow="9620" yWindow="3240" windowWidth="27640" windowHeight="16940" activeTab="3" xr2:uid="{52DA8E65-5893-DD4F-A6F9-F3DA94F38EDC}"/>
+    <workbookView xWindow="9720" yWindow="10240" windowWidth="27640" windowHeight="16940" xr2:uid="{52DA8E65-5893-DD4F-A6F9-F3DA94F38EDC}"/>
   </bookViews>
   <sheets>
-    <sheet name="Excretion" sheetId="1" r:id="rId1"/>
-    <sheet name="Toilet" sheetId="4" r:id="rId2"/>
-    <sheet name="PitLatrine" sheetId="5" r:id="rId3"/>
-    <sheet name="UDDT" sheetId="6" r:id="rId4"/>
+    <sheet name="Global" sheetId="8" r:id="rId1"/>
+    <sheet name="Excretion" sheetId="1" r:id="rId2"/>
+    <sheet name="Toilet" sheetId="4" r:id="rId3"/>
+    <sheet name="PitLatrine" sheetId="5" r:id="rId4"/>
+    <sheet name="UDDT" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,6 +38,49 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Yalin Li</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{863F58B8-1173-1D42-B55A-4718B750B768}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yalin Li:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Name for the corresponding parameters in another repository (https://github.com/QSD-for-WaSH/Bwaise-sanitation-alternatives)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Yalin Li</author>
@@ -79,7 +123,7 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Yalin Li</author>
@@ -122,7 +166,7 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Yalin Li</author>
@@ -240,7 +284,7 @@
 </comments>
 </file>
 
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Yalin Li</author>
@@ -358,7 +402,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="183">
   <si>
     <t>caloric_intake</t>
   </si>
@@ -894,6 +938,24 @@
   </si>
   <si>
     <t>moi_red_rate</t>
+  </si>
+  <si>
+    <t>time_full_degradation</t>
+  </si>
+  <si>
+    <t>reduction_full_degradation</t>
+  </si>
+  <si>
+    <t>log reduction</t>
+  </si>
+  <si>
+    <t>Assumption</t>
+  </si>
+  <si>
+    <t>tau_deg</t>
+  </si>
+  <si>
+    <t>log_deg</t>
   </si>
 </sst>
 </file>
@@ -1314,11 +1376,108 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{717F74A3-1EA7-BF4C-888F-570438234C81}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2">
+        <v>3</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D3" s="2">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2">
+        <v>2</v>
+      </c>
+      <c r="F3" s="2">
+        <v>4</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE7BC447-558C-1948-86CA-9891C0EAE965}">
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2018,12 +2177,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9909E3D-DD4D-2A48-BC53-FF96061B60F8}">
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2313,7 +2472,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{195BF460-1BB8-7A4C-B1C5-603B2E87D945}">
   <dimension ref="A1:J9"/>
   <sheetViews>
@@ -2561,11 +2720,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBDB86CE-4DA2-B346-BAA4-0E1F630CFBE6}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update Toilet, compelte PitLatrine design
</commit_message>
<xml_diff>
--- a/sanitation/systems/bwaise/inputs/units.xlsx
+++ b/sanitation/systems/bwaise/inputs/units.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfca01abaf64aab7/Coding/sanitation_Yalin/sanitation/systems/bwaise/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="561" documentId="8_{DCECA136-6458-0041-B737-5433DA0EAABB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E693DE9D-A6B5-764A-AFF2-2349CC8483AE}"/>
+  <xr:revisionPtr revIDLastSave="564" documentId="8_{DCECA136-6458-0041-B737-5433DA0EAABB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2FA06E5A-1371-B546-85E9-B9BD84B61ABA}"/>
   <bookViews>
-    <workbookView xWindow="9720" yWindow="10240" windowWidth="27640" windowHeight="16940" xr2:uid="{52DA8E65-5893-DD4F-A6F9-F3DA94F38EDC}"/>
+    <workbookView xWindow="10760" yWindow="1980" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{52DA8E65-5893-DD4F-A6F9-F3DA94F38EDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="8" r:id="rId1"/>
@@ -829,9 +829,6 @@
     <t>Orner and Mihelcic, 2017</t>
   </si>
   <si>
-    <t>N_removal</t>
-  </si>
-  <si>
     <t>MCF_aq</t>
   </si>
   <si>
@@ -844,9 +841,6 @@
     <t>N2O_EF_aquatic_discharge</t>
   </si>
   <si>
-    <t>COD_removal</t>
-  </si>
-  <si>
     <t>stored_urine_pH</t>
   </si>
   <si>
@@ -956,6 +950,12 @@
   </si>
   <si>
     <t>log_deg</t>
+  </si>
+  <si>
+    <t>COD_max_removal</t>
+  </si>
+  <si>
+    <t>N_max_removal</t>
   </si>
 </sst>
 </file>
@@ -1379,8 +1379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{717F74A3-1EA7-BF4C-888F-570438234C81}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1416,10 +1416,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C2" t="s">
         <v>132</v>
@@ -1437,18 +1437,18 @@
         <v>30</v>
       </c>
       <c r="H2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D3" s="2">
         <v>3</v>
@@ -1463,7 +1463,7 @@
         <v>30</v>
       </c>
       <c r="H3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -2181,13 +2181,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9909E3D-DD4D-2A48-BC53-FF96061B60F8}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
@@ -2364,7 +2364,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>145</v>
+        <v>181</v>
       </c>
       <c r="B7" t="s">
         <v>134</v>
@@ -2390,7 +2390,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>140</v>
+        <v>182</v>
       </c>
       <c r="B8" t="s">
         <v>136</v>
@@ -2416,10 +2416,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C9" t="s">
         <v>112</v>
@@ -2442,10 +2442,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C10" t="s">
         <v>110</v>
@@ -2679,7 +2679,7 @@
         <v>113</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>35</v>
@@ -2699,13 +2699,13 @@
         <v>110</v>
       </c>
       <c r="D9" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="F9" s="9" t="s">
         <v>168</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>170</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>30</v>
@@ -2792,10 +2792,10 @@
         <v>109</v>
       </c>
       <c r="B3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D3" s="2">
         <v>0.05</v>
@@ -2810,18 +2810,18 @@
         <v>30</v>
       </c>
       <c r="H3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D4" s="2">
         <v>7.57</v>
@@ -2836,18 +2836,18 @@
         <v>30</v>
       </c>
       <c r="H4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D5" s="2">
         <v>0.75</v>
@@ -2862,18 +2862,18 @@
         <v>30</v>
       </c>
       <c r="H5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D6" s="2">
         <v>2</v>
@@ -2888,18 +2888,18 @@
         <v>30</v>
       </c>
       <c r="H6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D7" s="2">
         <v>9</v>
@@ -2914,7 +2914,7 @@
         <v>30</v>
       </c>
       <c r="H7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -2922,7 +2922,7 @@
         <v>121</v>
       </c>
       <c r="B8" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C8" t="s">
         <v>112</v>
@@ -2948,7 +2948,7 @@
         <v>122</v>
       </c>
       <c r="B9" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C9" t="s">
         <v>110</v>
@@ -2971,10 +2971,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B10" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C10" t="s">
         <v>33</v>
@@ -2992,18 +2992,18 @@
         <v>30</v>
       </c>
       <c r="H10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B11" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C11" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D11" s="2">
         <v>0.01</v>
@@ -3018,7 +3018,7 @@
         <v>30</v>
       </c>
       <c r="H11" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
move Excretion, Toilet, PitLatrine, and UDDT to units
</commit_message>
<xml_diff>
--- a/sanitation/systems/bwaise/inputs/units.xlsx
+++ b/sanitation/systems/bwaise/inputs/units.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfca01abaf64aab7/Coding/sanitation_Yalin/sanitation/systems/bwaise/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="564" documentId="8_{DCECA136-6458-0041-B737-5433DA0EAABB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2FA06E5A-1371-B546-85E9-B9BD84B61ABA}"/>
+  <xr:revisionPtr revIDLastSave="567" documentId="8_{DCECA136-6458-0041-B737-5433DA0EAABB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6CBD121F-DEDC-A049-AD77-F64AFD8BFBA4}"/>
   <bookViews>
-    <workbookView xWindow="10760" yWindow="1980" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{52DA8E65-5893-DD4F-A6F9-F3DA94F38EDC}"/>
+    <workbookView xWindow="9080" yWindow="4960" windowWidth="27640" windowHeight="16940" activeTab="4" xr2:uid="{52DA8E65-5893-DD4F-A6F9-F3DA94F38EDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="8" r:id="rId1"/>
@@ -928,12 +928,6 @@
     <t>estimated using data from Niwagaba et al. (2009)</t>
   </si>
   <si>
-    <t>moi_min</t>
-  </si>
-  <si>
-    <t>moi_red_rate</t>
-  </si>
-  <si>
     <t>time_full_degradation</t>
   </si>
   <si>
@@ -956,6 +950,12 @@
   </si>
   <si>
     <t>N_max_removal</t>
+  </si>
+  <si>
+    <t>fec_moi_min</t>
+  </si>
+  <si>
+    <t>fec_moi_red_rate</t>
   </si>
 </sst>
 </file>
@@ -1416,10 +1416,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C2" t="s">
         <v>132</v>
@@ -1437,18 +1437,18 @@
         <v>30</v>
       </c>
       <c r="H2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D3" s="2">
         <v>3</v>
@@ -1463,7 +1463,7 @@
         <v>30</v>
       </c>
       <c r="H3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -2181,7 +2181,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9909E3D-DD4D-2A48-BC53-FF96061B60F8}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
@@ -2364,7 +2364,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B7" t="s">
         <v>134</v>
@@ -2390,7 +2390,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B8" t="s">
         <v>136</v>
@@ -2724,13 +2724,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBDB86CE-4DA2-B346-BAA4-0E1F630CFBE6}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.33203125" customWidth="1"/>
   </cols>
@@ -2971,7 +2971,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="B10" t="s">
         <v>169</v>
@@ -2997,7 +2997,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="B11" t="s">
         <v>170</v>

</xml_diff>